<commit_message>
Clean cell-by-cell aggregate data.
</commit_message>
<xml_diff>
--- a/2016-05-23_data/props.xlsx
+++ b/2016-05-23_data/props.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="All_chimeras_with_valid.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -33,12 +33,6 @@
     <t>GFP_std</t>
   </si>
   <si>
-    <t>GFP_mKate_cell</t>
-  </si>
-  <si>
-    <t>GFP_mKate_cell_std</t>
-  </si>
-  <si>
     <t>cell</t>
   </si>
   <si>
@@ -676,16 +670,38 @@
   </si>
   <si>
     <t>n8_2</t>
+  </si>
+  <si>
+    <t>cell_ratio</t>
+  </si>
+  <si>
+    <t>cell_ratio_std</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -708,13 +724,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1046,15 +1070,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
-      <selection activeCell="A216" sqref="A216"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1069,18 +1093,18 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>217</v>
+      </c>
+      <c r="G1" t="s">
+        <v>218</v>
+      </c>
+      <c r="H1" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>7.3029649999999998E-3</v>
@@ -1106,7 +1130,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>1.9082241E-2</v>
@@ -1132,7 +1156,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>2.8031430000000001E-3</v>
@@ -1158,7 +1182,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>5.640735E-3</v>
@@ -1184,7 +1208,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>7.5922359999999996E-3</v>
@@ -1210,7 +1234,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>1.4925388E-2</v>
@@ -1236,7 +1260,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8">
         <v>2.5506762999999998E-2</v>
@@ -1262,7 +1286,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <v>1.5018159E-2</v>
@@ -1288,7 +1312,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10">
         <v>6.6811969999999998E-3</v>
@@ -1314,7 +1338,7 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B11">
         <v>1.4866150999999999E-2</v>
@@ -1340,7 +1364,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>4.012046E-3</v>
@@ -1366,7 +1390,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>3.8033580000000002E-3</v>
@@ -1392,7 +1416,7 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B14">
         <v>1.1482282999999999E-2</v>
@@ -1418,7 +1442,7 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B15">
         <v>7.6951720000000001E-3</v>
@@ -1444,7 +1468,7 @@
     </row>
     <row r="16" spans="1:8">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16">
         <v>3.787487E-3</v>
@@ -1470,7 +1494,7 @@
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B17">
         <v>2.84338E-3</v>
@@ -1496,7 +1520,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <v>1.277436E-2</v>
@@ -1522,7 +1546,7 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B19">
         <v>3.4657910000000002E-3</v>
@@ -1548,7 +1572,7 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B20">
         <v>9.4318509999999998E-3</v>
@@ -1574,7 +1598,7 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B21">
         <v>6.0686749999999999E-3</v>
@@ -1600,7 +1624,7 @@
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B22">
         <v>5.6011129999999996E-3</v>
@@ -1626,7 +1650,7 @@
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B23">
         <v>4.5523839999999996E-3</v>
@@ -1652,7 +1676,7 @@
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B24">
         <v>7.1407290000000002E-3</v>
@@ -1678,7 +1702,7 @@
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B25">
         <v>8.8119340000000004E-3</v>
@@ -1704,7 +1728,7 @@
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26">
         <v>1.5490314E-2</v>
@@ -1730,7 +1754,7 @@
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>2.8343589999999998E-3</v>
@@ -1756,7 +1780,7 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B28">
         <v>9.2677530000000001E-3</v>
@@ -1782,7 +1806,7 @@
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B29">
         <v>3.7165409999999999E-3</v>
@@ -1808,7 +1832,7 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B30">
         <v>6.9793479999999998E-3</v>
@@ -1834,7 +1858,7 @@
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B31">
         <v>2.8320760000000002E-3</v>
@@ -1860,7 +1884,7 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B32">
         <v>1.8097480999999999E-2</v>
@@ -1886,7 +1910,7 @@
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B33">
         <v>6.4192650000000004E-3</v>
@@ -1912,7 +1936,7 @@
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B34">
         <v>4.2663010000000001E-3</v>
@@ -1938,7 +1962,7 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B35">
         <v>2.4186467E-2</v>
@@ -1964,7 +1988,7 @@
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B36">
         <v>2.3636458999999999E-2</v>
@@ -1990,7 +2014,7 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B37">
         <v>2.0271127E-2</v>
@@ -2016,7 +2040,7 @@
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B38">
         <v>1.2497022E-2</v>
@@ -2042,7 +2066,7 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B39">
         <v>3.004535E-3</v>
@@ -2068,7 +2092,7 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B40">
         <v>1.1781603999999999E-2</v>
@@ -2094,7 +2118,7 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B41">
         <v>4.6709789999999996E-3</v>
@@ -2120,7 +2144,7 @@
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B42">
         <v>7.2224589999999997E-3</v>
@@ -2146,7 +2170,7 @@
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B43">
         <v>4.2510489999999998E-3</v>
@@ -2172,7 +2196,7 @@
     </row>
     <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B44">
         <v>1.1957140999999999E-2</v>
@@ -2198,7 +2222,7 @@
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B45">
         <v>2.1347551999999999E-2</v>
@@ -2224,7 +2248,7 @@
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B46">
         <v>1.0984437E-2</v>
@@ -2250,7 +2274,7 @@
     </row>
     <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B47">
         <v>1.1836073000000001E-2</v>
@@ -2276,7 +2300,7 @@
     </row>
     <row r="48" spans="1:8">
       <c r="A48" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B48">
         <v>7.2702909999999999E-3</v>
@@ -2302,7 +2326,7 @@
     </row>
     <row r="49" spans="1:8">
       <c r="A49" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B49">
         <v>6.153525E-3</v>
@@ -2328,7 +2352,7 @@
     </row>
     <row r="50" spans="1:8">
       <c r="A50" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B50">
         <v>1.2553923999999999E-2</v>
@@ -2354,7 +2378,7 @@
     </row>
     <row r="51" spans="1:8">
       <c r="A51" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B51">
         <v>1.4228502000000001E-2</v>
@@ -2380,7 +2404,7 @@
     </row>
     <row r="52" spans="1:8">
       <c r="A52" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B52">
         <v>1.1014569E-2</v>
@@ -2406,7 +2430,7 @@
     </row>
     <row r="53" spans="1:8">
       <c r="A53" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B53">
         <v>8.3782470000000001E-3</v>
@@ -2432,7 +2456,7 @@
     </row>
     <row r="54" spans="1:8">
       <c r="A54" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B54">
         <v>1.2039665E-2</v>
@@ -2458,7 +2482,7 @@
     </row>
     <row r="55" spans="1:8">
       <c r="A55" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B55">
         <v>1.8221244000000001E-2</v>
@@ -2484,7 +2508,7 @@
     </row>
     <row r="56" spans="1:8">
       <c r="A56" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B56">
         <v>1.8249850000000001E-2</v>
@@ -2510,7 +2534,7 @@
     </row>
     <row r="57" spans="1:8">
       <c r="A57" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B57">
         <v>1.3453781E-2</v>
@@ -2536,7 +2560,7 @@
     </row>
     <row r="58" spans="1:8">
       <c r="A58" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B58">
         <v>1.8065939E-2</v>
@@ -2562,7 +2586,7 @@
     </row>
     <row r="59" spans="1:8">
       <c r="A59" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B59">
         <v>8.5137939999999999E-3</v>
@@ -2588,7 +2612,7 @@
     </row>
     <row r="60" spans="1:8">
       <c r="A60" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B60">
         <v>3.9893919999999996E-3</v>
@@ -2614,7 +2638,7 @@
     </row>
     <row r="61" spans="1:8">
       <c r="A61" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B61">
         <v>7.3534259999999997E-3</v>
@@ -2640,7 +2664,7 @@
     </row>
     <row r="62" spans="1:8">
       <c r="A62" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B62">
         <v>7.4543600000000002E-3</v>
@@ -2666,7 +2690,7 @@
     </row>
     <row r="63" spans="1:8">
       <c r="A63" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B63">
         <v>4.7558990000000001E-3</v>
@@ -2692,7 +2716,7 @@
     </row>
     <row r="64" spans="1:8">
       <c r="A64" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B64">
         <v>5.2869019999999996E-3</v>
@@ -2718,7 +2742,7 @@
     </row>
     <row r="65" spans="1:8">
       <c r="A65" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B65">
         <v>3.107898E-3</v>
@@ -2744,7 +2768,7 @@
     </row>
     <row r="66" spans="1:8">
       <c r="A66" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B66">
         <v>5.1402039999999998E-3</v>
@@ -2770,7 +2794,7 @@
     </row>
     <row r="67" spans="1:8">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B67">
         <v>2.8269689999999999E-3</v>
@@ -2796,7 +2820,7 @@
     </row>
     <row r="68" spans="1:8">
       <c r="A68" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B68">
         <v>2.9284390000000001E-3</v>
@@ -2822,7 +2846,7 @@
     </row>
     <row r="69" spans="1:8">
       <c r="A69" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B69">
         <v>8.8870080000000001E-3</v>
@@ -2848,7 +2872,7 @@
     </row>
     <row r="70" spans="1:8">
       <c r="A70" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B70">
         <v>5.668948E-3</v>
@@ -2874,7 +2898,7 @@
     </row>
     <row r="71" spans="1:8">
       <c r="A71" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B71">
         <v>1.3975313E-2</v>
@@ -2900,7 +2924,7 @@
     </row>
     <row r="72" spans="1:8">
       <c r="A72" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B72">
         <v>7.3652609999999997E-3</v>
@@ -2926,7 +2950,7 @@
     </row>
     <row r="73" spans="1:8">
       <c r="A73" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B73">
         <v>4.1631719999999997E-3</v>
@@ -2952,7 +2976,7 @@
     </row>
     <row r="74" spans="1:8">
       <c r="A74" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B74">
         <v>3.6841410000000002E-3</v>
@@ -2978,7 +3002,7 @@
     </row>
     <row r="75" spans="1:8">
       <c r="A75" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B75">
         <v>4.5802969999999997E-3</v>
@@ -3004,7 +3028,7 @@
     </row>
     <row r="76" spans="1:8">
       <c r="A76" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B76">
         <v>1.6508793000000001E-2</v>
@@ -3030,7 +3054,7 @@
     </row>
     <row r="77" spans="1:8">
       <c r="A77" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B77">
         <v>7.404379E-3</v>
@@ -3056,7 +3080,7 @@
     </row>
     <row r="78" spans="1:8">
       <c r="A78" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B78">
         <v>4.9662580000000003E-3</v>
@@ -3082,7 +3106,7 @@
     </row>
     <row r="79" spans="1:8">
       <c r="A79" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B79">
         <v>3.2577890000000001E-3</v>
@@ -3108,7 +3132,7 @@
     </row>
     <row r="80" spans="1:8">
       <c r="A80" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B80">
         <v>5.5095589999999998E-3</v>
@@ -3134,7 +3158,7 @@
     </row>
     <row r="81" spans="1:8">
       <c r="A81" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B81">
         <v>1.3162003E-2</v>
@@ -3160,7 +3184,7 @@
     </row>
     <row r="82" spans="1:8">
       <c r="A82" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B82">
         <v>7.9073059999999994E-3</v>
@@ -3186,7 +3210,7 @@
     </row>
     <row r="83" spans="1:8">
       <c r="A83" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B83">
         <v>7.0934350000000004E-3</v>
@@ -3212,7 +3236,7 @@
     </row>
     <row r="84" spans="1:8">
       <c r="A84" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B84">
         <v>2.1679295000000001E-2</v>
@@ -3238,7 +3262,7 @@
     </row>
     <row r="85" spans="1:8">
       <c r="A85" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B85">
         <v>5.8796459999999997E-3</v>
@@ -3264,7 +3288,7 @@
     </row>
     <row r="86" spans="1:8">
       <c r="A86" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B86">
         <v>1.3724114000000001E-2</v>
@@ -3290,7 +3314,7 @@
     </row>
     <row r="87" spans="1:8">
       <c r="A87" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B87">
         <v>9.6589450000000004E-3</v>
@@ -3316,7 +3340,7 @@
     </row>
     <row r="88" spans="1:8">
       <c r="A88" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B88">
         <v>9.6197460000000002E-3</v>
@@ -3342,7 +3366,7 @@
     </row>
     <row r="89" spans="1:8">
       <c r="A89" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B89">
         <v>4.8253979999999998E-3</v>
@@ -3368,7 +3392,7 @@
     </row>
     <row r="90" spans="1:8">
       <c r="A90" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B90">
         <v>4.5583059999999998E-3</v>
@@ -3394,7 +3418,7 @@
     </row>
     <row r="91" spans="1:8">
       <c r="A91" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B91">
         <v>8.3978400000000002E-3</v>
@@ -3420,7 +3444,7 @@
     </row>
     <row r="92" spans="1:8">
       <c r="A92" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B92">
         <v>1.0946997E-2</v>
@@ -3446,7 +3470,7 @@
     </row>
     <row r="93" spans="1:8">
       <c r="A93" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B93">
         <v>1.2789716E-2</v>
@@ -3472,7 +3496,7 @@
     </row>
     <row r="94" spans="1:8">
       <c r="A94" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B94">
         <v>1.2233536999999999E-2</v>
@@ -3498,7 +3522,7 @@
     </row>
     <row r="95" spans="1:8">
       <c r="A95" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B95">
         <v>2.858335E-3</v>
@@ -3524,7 +3548,7 @@
     </row>
     <row r="96" spans="1:8">
       <c r="A96" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B96">
         <v>1.9235782999999999E-2</v>
@@ -3550,7 +3574,7 @@
     </row>
     <row r="97" spans="1:8">
       <c r="A97" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B97">
         <v>5.548023E-3</v>
@@ -3576,7 +3600,7 @@
     </row>
     <row r="98" spans="1:8">
       <c r="A98" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B98">
         <v>2.934313E-3</v>
@@ -3602,7 +3626,7 @@
     </row>
     <row r="99" spans="1:8">
       <c r="A99" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B99">
         <v>4.1919640000000003E-3</v>
@@ -3628,7 +3652,7 @@
     </row>
     <row r="100" spans="1:8">
       <c r="A100" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B100">
         <v>9.8648599999999996E-3</v>
@@ -3654,7 +3678,7 @@
     </row>
     <row r="101" spans="1:8">
       <c r="A101" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B101">
         <v>6.3207580000000001E-3</v>
@@ -3680,7 +3704,7 @@
     </row>
     <row r="102" spans="1:8">
       <c r="A102" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B102">
         <v>6.972247E-3</v>
@@ -3706,7 +3730,7 @@
     </row>
     <row r="103" spans="1:8">
       <c r="A103" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B103">
         <v>1.2237827999999999E-2</v>
@@ -3732,7 +3756,7 @@
     </row>
     <row r="104" spans="1:8">
       <c r="A104" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B104">
         <v>5.2438889999999998E-3</v>
@@ -3758,7 +3782,7 @@
     </row>
     <row r="105" spans="1:8">
       <c r="A105" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B105">
         <v>6.0270130000000003E-3</v>
@@ -3784,7 +3808,7 @@
     </row>
     <row r="106" spans="1:8">
       <c r="A106" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B106">
         <v>4.7992180000000001E-3</v>
@@ -3810,7 +3834,7 @@
     </row>
     <row r="107" spans="1:8">
       <c r="A107" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B107">
         <v>1.3752283000000001E-2</v>
@@ -3836,7 +3860,7 @@
     </row>
     <row r="108" spans="1:8">
       <c r="A108" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B108">
         <v>1.1126495E-2</v>
@@ -3862,7 +3886,7 @@
     </row>
     <row r="109" spans="1:8">
       <c r="A109" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B109">
         <v>1.6266022000000002E-2</v>
@@ -3888,7 +3912,7 @@
     </row>
     <row r="110" spans="1:8">
       <c r="A110" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B110">
         <v>4.7638890000000003E-3</v>
@@ -3914,7 +3938,7 @@
     </row>
     <row r="111" spans="1:8">
       <c r="A111" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B111">
         <v>4.0042630000000001E-3</v>
@@ -3940,7 +3964,7 @@
     </row>
     <row r="112" spans="1:8">
       <c r="A112" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B112">
         <v>1.4405569E-2</v>
@@ -3966,7 +3990,7 @@
     </row>
     <row r="113" spans="1:8">
       <c r="A113" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B113">
         <v>1.8945855000000001E-2</v>
@@ -3992,7 +4016,7 @@
     </row>
     <row r="114" spans="1:8">
       <c r="A114" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B114">
         <v>9.8604529999999999E-3</v>
@@ -4018,7 +4042,7 @@
     </row>
     <row r="115" spans="1:8">
       <c r="A115" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B115">
         <v>1.1061893E-2</v>
@@ -4044,7 +4068,7 @@
     </row>
     <row r="116" spans="1:8">
       <c r="A116" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B116">
         <v>4.2110020000000001E-3</v>
@@ -4070,7 +4094,7 @@
     </row>
     <row r="117" spans="1:8">
       <c r="A117" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B117">
         <v>6.7492070000000001E-3</v>
@@ -4096,7 +4120,7 @@
     </row>
     <row r="118" spans="1:8">
       <c r="A118" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B118">
         <v>4.3513320000000003E-3</v>
@@ -4122,7 +4146,7 @@
     </row>
     <row r="119" spans="1:8">
       <c r="A119" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B119">
         <v>4.3500190000000001E-3</v>
@@ -4148,7 +4172,7 @@
     </row>
     <row r="120" spans="1:8">
       <c r="A120" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B120">
         <v>5.5782039999999998E-3</v>
@@ -4174,7 +4198,7 @@
     </row>
     <row r="121" spans="1:8">
       <c r="A121" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B121">
         <v>1.1961565E-2</v>
@@ -4200,7 +4224,7 @@
     </row>
     <row r="122" spans="1:8">
       <c r="A122" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B122">
         <v>1.1476139E-2</v>
@@ -4226,7 +4250,7 @@
     </row>
     <row r="123" spans="1:8">
       <c r="A123" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B123">
         <v>6.898103E-3</v>
@@ -4252,7 +4276,7 @@
     </row>
     <row r="124" spans="1:8">
       <c r="A124" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B124">
         <v>6.050176E-3</v>
@@ -4278,7 +4302,7 @@
     </row>
     <row r="125" spans="1:8">
       <c r="A125" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B125">
         <v>4.9976020000000003E-3</v>
@@ -4304,7 +4328,7 @@
     </row>
     <row r="126" spans="1:8">
       <c r="A126" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B126">
         <v>3.8600589999999999E-3</v>
@@ -4330,7 +4354,7 @@
     </row>
     <row r="127" spans="1:8">
       <c r="A127" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B127">
         <v>5.0498979999999997E-3</v>
@@ -4356,7 +4380,7 @@
     </row>
     <row r="128" spans="1:8">
       <c r="A128" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B128">
         <v>3.9738730000000002E-3</v>
@@ -4382,7 +4406,7 @@
     </row>
     <row r="129" spans="1:8">
       <c r="A129" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B129">
         <v>3.9113489999999997E-3</v>
@@ -4408,7 +4432,7 @@
     </row>
     <row r="130" spans="1:8">
       <c r="A130" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B130">
         <v>4.5772199999999999E-3</v>
@@ -4434,7 +4458,7 @@
     </row>
     <row r="131" spans="1:8">
       <c r="A131" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B131">
         <v>3.6765209999999999E-3</v>
@@ -4460,7 +4484,7 @@
     </row>
     <row r="132" spans="1:8">
       <c r="A132" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B132">
         <v>5.0946289999999998E-3</v>
@@ -4486,7 +4510,7 @@
     </row>
     <row r="133" spans="1:8">
       <c r="A133" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B133">
         <v>5.3786750000000003E-3</v>
@@ -4512,7 +4536,7 @@
     </row>
     <row r="134" spans="1:8">
       <c r="A134" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B134">
         <v>1.0322753E-2</v>
@@ -4538,7 +4562,7 @@
     </row>
     <row r="135" spans="1:8">
       <c r="A135" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B135">
         <v>1.5675529000000001E-2</v>
@@ -4564,7 +4588,7 @@
     </row>
     <row r="136" spans="1:8">
       <c r="A136" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B136">
         <v>1.2449302000000001E-2</v>
@@ -4590,7 +4614,7 @@
     </row>
     <row r="137" spans="1:8">
       <c r="A137" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B137">
         <v>6.670507E-3</v>
@@ -4616,7 +4640,7 @@
     </row>
     <row r="138" spans="1:8">
       <c r="A138" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B138">
         <v>8.9314930000000004E-3</v>
@@ -4642,7 +4666,7 @@
     </row>
     <row r="139" spans="1:8">
       <c r="A139" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B139">
         <v>1.3987124E-2</v>
@@ -4668,7 +4692,7 @@
     </row>
     <row r="140" spans="1:8">
       <c r="A140" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B140">
         <v>1.2145972999999999E-2</v>
@@ -4694,7 +4718,7 @@
     </row>
     <row r="141" spans="1:8">
       <c r="A141" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B141">
         <v>1.1009433000000001E-2</v>
@@ -4720,7 +4744,7 @@
     </row>
     <row r="142" spans="1:8">
       <c r="A142" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B142">
         <v>4.1199499999999998E-3</v>
@@ -4746,7 +4770,7 @@
     </row>
     <row r="143" spans="1:8">
       <c r="A143" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B143">
         <v>6.1851479999999997E-3</v>
@@ -4772,7 +4796,7 @@
     </row>
     <row r="144" spans="1:8">
       <c r="A144" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B144">
         <v>3.9437049999999996E-3</v>
@@ -4798,7 +4822,7 @@
     </row>
     <row r="145" spans="1:8">
       <c r="A145" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B145">
         <v>3.8239279999999999E-3</v>
@@ -4824,7 +4848,7 @@
     </row>
     <row r="146" spans="1:8">
       <c r="A146" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B146">
         <v>4.7177959999999998E-3</v>
@@ -4850,7 +4874,7 @@
     </row>
     <row r="147" spans="1:8">
       <c r="A147" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B147">
         <v>5.1998720000000003E-3</v>
@@ -4876,7 +4900,7 @@
     </row>
     <row r="148" spans="1:8">
       <c r="A148" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B148">
         <v>3.1733460000000001E-3</v>
@@ -4902,7 +4926,7 @@
     </row>
     <row r="149" spans="1:8">
       <c r="A149" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B149">
         <v>3.9966280000000003E-3</v>
@@ -4928,7 +4952,7 @@
     </row>
     <row r="150" spans="1:8">
       <c r="A150" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B150">
         <v>5.0192830000000003E-3</v>
@@ -4954,7 +4978,7 @@
     </row>
     <row r="151" spans="1:8">
       <c r="A151" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B151">
         <v>4.8791700000000004E-3</v>
@@ -4980,7 +5004,7 @@
     </row>
     <row r="152" spans="1:8">
       <c r="A152" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B152">
         <v>1.2628393999999999E-2</v>
@@ -5006,7 +5030,7 @@
     </row>
     <row r="153" spans="1:8">
       <c r="A153" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B153">
         <v>1.2247628E-2</v>
@@ -5032,7 +5056,7 @@
     </row>
     <row r="154" spans="1:8">
       <c r="A154" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B154">
         <v>1.0475622E-2</v>
@@ -5058,7 +5082,7 @@
     </row>
     <row r="155" spans="1:8">
       <c r="A155" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B155">
         <v>1.2988497E-2</v>
@@ -5084,7 +5108,7 @@
     </row>
     <row r="156" spans="1:8">
       <c r="A156" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B156">
         <v>3.0940859999999998E-3</v>
@@ -5110,7 +5134,7 @@
     </row>
     <row r="157" spans="1:8">
       <c r="A157" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B157">
         <v>5.7930509999999996E-3</v>
@@ -5136,7 +5160,7 @@
     </row>
     <row r="158" spans="1:8">
       <c r="A158" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B158">
         <v>4.7093150000000004E-3</v>
@@ -5162,7 +5186,7 @@
     </row>
     <row r="159" spans="1:8">
       <c r="A159" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B159">
         <v>4.9119489999999997E-3</v>
@@ -5188,7 +5212,7 @@
     </row>
     <row r="160" spans="1:8">
       <c r="A160" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B160">
         <v>9.6766869999999998E-3</v>
@@ -5214,7 +5238,7 @@
     </row>
     <row r="161" spans="1:8">
       <c r="A161" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B161">
         <v>7.978054E-3</v>
@@ -5240,7 +5264,7 @@
     </row>
     <row r="162" spans="1:8">
       <c r="A162" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B162">
         <v>2.5345349999999999E-2</v>
@@ -5266,7 +5290,7 @@
     </row>
     <row r="163" spans="1:8">
       <c r="A163" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B163">
         <v>1.1376054E-2</v>
@@ -5292,7 +5316,7 @@
     </row>
     <row r="164" spans="1:8">
       <c r="A164" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B164">
         <v>1.0860450000000001E-2</v>
@@ -5318,7 +5342,7 @@
     </row>
     <row r="165" spans="1:8">
       <c r="A165" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B165">
         <v>7.5200470000000002E-3</v>
@@ -5344,7 +5368,7 @@
     </row>
     <row r="166" spans="1:8">
       <c r="A166" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B166">
         <v>1.2820444E-2</v>
@@ -5370,7 +5394,7 @@
     </row>
     <row r="167" spans="1:8">
       <c r="A167" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B167">
         <v>6.4137480000000004E-3</v>
@@ -5396,7 +5420,7 @@
     </row>
     <row r="168" spans="1:8">
       <c r="A168" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B168">
         <v>6.4957649999999997E-3</v>
@@ -5422,7 +5446,7 @@
     </row>
     <row r="169" spans="1:8">
       <c r="A169" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B169">
         <v>1.429123E-2</v>
@@ -5448,7 +5472,7 @@
     </row>
     <row r="170" spans="1:8">
       <c r="A170" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B170">
         <v>5.3090730000000001E-3</v>
@@ -5474,7 +5498,7 @@
     </row>
     <row r="171" spans="1:8">
       <c r="A171" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B171">
         <v>1.0578547000000001E-2</v>
@@ -5500,7 +5524,7 @@
     </row>
     <row r="172" spans="1:8">
       <c r="A172" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B172">
         <v>5.5146589999999999E-3</v>
@@ -5526,7 +5550,7 @@
     </row>
     <row r="173" spans="1:8">
       <c r="A173" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B173">
         <v>2.8441370000000001E-3</v>
@@ -5552,7 +5576,7 @@
     </row>
     <row r="174" spans="1:8">
       <c r="A174" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B174">
         <v>1.6951713E-2</v>
@@ -5578,7 +5602,7 @@
     </row>
     <row r="175" spans="1:8">
       <c r="A175" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B175">
         <v>4.1522429999999999E-3</v>
@@ -5604,7 +5628,7 @@
     </row>
     <row r="176" spans="1:8">
       <c r="A176" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B176">
         <v>1.6849191999999999E-2</v>
@@ -5630,7 +5654,7 @@
     </row>
     <row r="177" spans="1:8">
       <c r="A177" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B177">
         <v>8.2819209999999994E-3</v>
@@ -5656,7 +5680,7 @@
     </row>
     <row r="178" spans="1:8">
       <c r="A178" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B178">
         <v>2.978138E-3</v>
@@ -5682,7 +5706,7 @@
     </row>
     <row r="179" spans="1:8">
       <c r="A179" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B179">
         <v>3.7125399999999999E-3</v>
@@ -5708,7 +5732,7 @@
     </row>
     <row r="180" spans="1:8">
       <c r="A180" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B180">
         <v>3.3827839999999998E-3</v>
@@ -5734,7 +5758,7 @@
     </row>
     <row r="181" spans="1:8">
       <c r="A181" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B181">
         <v>6.1081529999999998E-3</v>
@@ -5760,7 +5784,7 @@
     </row>
     <row r="182" spans="1:8">
       <c r="A182" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B182">
         <v>1.0955166000000001E-2</v>
@@ -5786,7 +5810,7 @@
     </row>
     <row r="183" spans="1:8">
       <c r="A183" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B183">
         <v>4.8390229999999996E-3</v>
@@ -5812,7 +5836,7 @@
     </row>
     <row r="184" spans="1:8">
       <c r="A184" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B184">
         <v>1.1447362000000001E-2</v>
@@ -5838,7 +5862,7 @@
     </row>
     <row r="185" spans="1:8">
       <c r="A185" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B185">
         <v>1.2585130999999999E-2</v>
@@ -5864,7 +5888,7 @@
     </row>
     <row r="186" spans="1:8">
       <c r="A186" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B186">
         <v>1.3551063E-2</v>
@@ -5890,7 +5914,7 @@
     </row>
     <row r="187" spans="1:8">
       <c r="A187" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B187">
         <v>3.0666619999999999E-3</v>
@@ -5916,7 +5940,7 @@
     </row>
     <row r="188" spans="1:8">
       <c r="A188" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B188">
         <v>3.7149729999999999E-3</v>
@@ -5942,7 +5966,7 @@
     </row>
     <row r="189" spans="1:8">
       <c r="A189" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B189">
         <v>1.0265774E-2</v>
@@ -5968,7 +5992,7 @@
     </row>
     <row r="190" spans="1:8">
       <c r="A190" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B190">
         <v>1.9279556E-2</v>
@@ -5994,7 +6018,7 @@
     </row>
     <row r="191" spans="1:8">
       <c r="A191" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B191">
         <v>6.2561869999999999E-3</v>
@@ -6020,7 +6044,7 @@
     </row>
     <row r="192" spans="1:8">
       <c r="A192" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B192">
         <v>7.7268989999999997E-3</v>
@@ -6046,7 +6070,7 @@
     </row>
     <row r="193" spans="1:8">
       <c r="A193" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B193">
         <v>2.0493912E-2</v>
@@ -6072,7 +6096,7 @@
     </row>
     <row r="194" spans="1:8">
       <c r="A194" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B194">
         <v>2.1502925999999999E-2</v>
@@ -6098,7 +6122,7 @@
     </row>
     <row r="195" spans="1:8">
       <c r="A195" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B195">
         <v>1.1644177E-2</v>
@@ -6124,7 +6148,7 @@
     </row>
     <row r="196" spans="1:8">
       <c r="A196" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B196">
         <v>2.4069411999999998E-2</v>
@@ -6150,7 +6174,7 @@
     </row>
     <row r="197" spans="1:8">
       <c r="A197" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B197">
         <v>1.7634378999999999E-2</v>
@@ -6176,7 +6200,7 @@
     </row>
     <row r="198" spans="1:8">
       <c r="A198" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B198">
         <v>6.3464940000000003E-3</v>
@@ -6202,7 +6226,7 @@
     </row>
     <row r="199" spans="1:8">
       <c r="A199" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B199">
         <v>9.4156229999999997E-3</v>
@@ -6228,7 +6252,7 @@
     </row>
     <row r="200" spans="1:8">
       <c r="A200" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B200">
         <v>1.3009148999999999E-2</v>
@@ -6254,7 +6278,7 @@
     </row>
     <row r="201" spans="1:8">
       <c r="A201" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B201">
         <v>1.6429915999999999E-2</v>
@@ -6280,7 +6304,7 @@
     </row>
     <row r="202" spans="1:8">
       <c r="A202" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B202">
         <v>1.2997681000000001E-2</v>
@@ -6306,7 +6330,7 @@
     </row>
     <row r="203" spans="1:8">
       <c r="A203" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B203">
         <v>3.126331E-3</v>
@@ -6332,7 +6356,7 @@
     </row>
     <row r="204" spans="1:8">
       <c r="A204" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B204">
         <v>8.8404940000000008E-3</v>
@@ -6358,7 +6382,7 @@
     </row>
     <row r="205" spans="1:8">
       <c r="A205" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B205">
         <v>9.6443180000000007E-3</v>
@@ -6384,7 +6408,7 @@
     </row>
     <row r="206" spans="1:8">
       <c r="A206" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B206">
         <v>8.7747269999999995E-3</v>
@@ -6410,7 +6434,7 @@
     </row>
     <row r="207" spans="1:8">
       <c r="A207" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B207">
         <v>1.021357E-2</v>
@@ -6436,7 +6460,7 @@
     </row>
     <row r="208" spans="1:8">
       <c r="A208" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B208">
         <v>6.5390880000000002E-3</v>
@@ -6462,7 +6486,7 @@
     </row>
     <row r="209" spans="1:8">
       <c r="A209" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B209">
         <v>9.7587799999999999E-3</v>
@@ -6488,7 +6512,7 @@
     </row>
     <row r="210" spans="1:8">
       <c r="A210" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B210">
         <v>1.6558519000000001E-2</v>
@@ -6514,7 +6538,7 @@
     </row>
     <row r="211" spans="1:8">
       <c r="A211" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B211">
         <v>1.0255172E-2</v>
@@ -6540,7 +6564,7 @@
     </row>
     <row r="212" spans="1:8">
       <c r="A212" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B212">
         <v>1.3958826000000001E-2</v>
@@ -6566,6 +6590,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>